<commit_message>
update on PA data and event taging
</commit_message>
<xml_diff>
--- a/Vale/Docs/ExistingPITag/PI_Tag_Resume.xlsx
+++ b/Vale/Docs/ExistingPITag/PI_Tag_Resume.xlsx
@@ -11484,8 +11484,8 @@
   </sheetPr>
   <dimension ref="A1:H372"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A331" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G361" activeCellId="0" sqref="G361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>